<commit_message>
fix in sanofiSA template
</commit_message>
<xml_diff>
--- a/Projects/SANOFISA/Data/Template.xlsx
+++ b/Projects/SANOFISA/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -137,6 +137,21 @@
         </r>
       </text>
     </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Indicate 1 for MSL / indicate 0 if not in MSL
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -212,6 +227,21 @@
       </text>
     </comment>
     <comment ref="F2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">Indicate 1 for MSL / indicate 0 if not in MSL
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -658,7 +688,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="81">
   <si>
     <t xml:space="preserve">KPI Name</t>
   </si>
@@ -777,6 +807,18 @@
     <t xml:space="preserve">CAT4</t>
   </si>
   <si>
+    <t xml:space="preserve">CAT1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAT2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAT3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAT4.1</t>
+  </si>
+  <si>
     <t xml:space="preserve">DULCOLAXSUCTA/ 30/5MG BLI KSA</t>
   </si>
   <si>
@@ -865,18 +907,6 @@
   </si>
   <si>
     <t xml:space="preserve">SKUs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAT1.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAT2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAT3.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CAT4.1</t>
   </si>
   <si>
     <t xml:space="preserve">PHARMATON SECONDARY</t>
@@ -1236,7 +1266,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="74">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1357,10 +1387,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1423,10 +1449,6 @@
     </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1621,20 +1643,20 @@
   </sheetPr>
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I9" activeCellId="1" sqref="J2:M2 I9"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4655870445344"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3036437246964"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0769230769231"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81376518218623"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.2591093117409"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.6882591093117"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="20.1943319838057"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3238866396761"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.7975708502024"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.8097165991903"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="26.080971659919"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.18218623481781"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1891,21 +1913,21 @@
   </sheetPr>
   <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="1" sqref="J2:M2 A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M32" activeCellId="0" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.336032388664"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="49.8259109311741"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.1174089068826"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="17.3805668016194"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="13" width="11.9959514170041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="9.06072874493927"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="22.1578947368421"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="14" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="52.2753036437247"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="23.2591093117409"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="18.1174089068826"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="13" width="12.4817813765182"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="9.30364372469636"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="14" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="14" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1920,9 +1942,12 @@
       <c r="G1" s="16"/>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
+      <c r="J1" s="0"/>
       <c r="K1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -1950,23 +1975,34 @@
       <c r="I2" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="K2" s="0"/>
+      <c r="J2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="19" t="s">
         <v>23</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F3" s="24" t="n">
         <v>1</v>
@@ -1998,16 +2034,16 @@
         <v>23</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C4" s="21" t="n">
         <v>3582910032373</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F4" s="24" t="n">
         <v>1</v>
@@ -2039,16 +2075,16 @@
         <v>23</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C5" s="21" t="n">
         <v>3582910034988</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F5" s="24" t="n">
         <v>1</v>
@@ -2080,16 +2116,16 @@
         <v>23</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="E6" s="26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F6" s="24" t="n">
         <v>1</v>
@@ -2121,16 +2157,16 @@
         <v>23</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C7" s="21" t="n">
         <v>201513619</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F7" s="24" t="n">
         <v>1</v>
@@ -2162,16 +2198,16 @@
         <v>23</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F8" s="24" t="n">
         <v>1</v>
@@ -2203,16 +2239,16 @@
         <v>23</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="F9" s="24" t="n">
         <v>0</v>
@@ -2244,16 +2280,16 @@
         <v>23</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="F10" s="24" t="n">
         <v>1</v>
@@ -2285,16 +2321,16 @@
         <v>23</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C11" s="21" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="D11" s="27" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E11" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F11" s="24" t="n">
         <v>1</v>
@@ -2326,16 +2362,16 @@
         <v>23</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="C12" s="21" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="D12" s="27" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="E12" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="F12" s="24" t="n">
         <v>1</v>
@@ -2382,37 +2418,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:M6"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D22" activeCellId="1" sqref="J2:M2 D22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J9" activeCellId="0" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="25.336032388664"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="28" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="28" width="31.3441295546559"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="21.4251012145749"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="28" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="29" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="30" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="26.5668016194332"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="28" width="22.4008097165992"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="28" width="32.9271255060729"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="28" width="22.4008097165992"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="28" width="11.6315789473684"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="29" width="11.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="14" width="9.30364372469636"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="32" t="s">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -2423,7 +2459,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="E2" s="17" t="s">
         <v>32</v>
@@ -2440,14 +2476,26 @@
       <c r="I2" s="18" t="s">
         <v>38</v>
       </c>
+      <c r="J2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="33" t="s">
+      <c r="A3" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="35"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="34"/>
       <c r="E3" s="13"/>
       <c r="F3" s="24"/>
       <c r="G3" s="24"/>
@@ -2455,36 +2503,36 @@
       <c r="I3" s="24"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="33" t="s">
+      <c r="A4" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
       <c r="F4" s="24"/>
       <c r="G4" s="24"/>
       <c r="H4" s="24"/>
       <c r="I4" s="24"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
+      <c r="A5" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="36"/>
       <c r="F5" s="24"/>
       <c r="G5" s="24"/>
       <c r="H5" s="24"/>
       <c r="I5" s="24"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="33" t="s">
+      <c r="A6" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="36"/>
       <c r="F6" s="24"/>
       <c r="G6" s="24"/>
       <c r="H6" s="24"/>
@@ -2512,34 +2560,38 @@
   </sheetPr>
   <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:M2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="38" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="38" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="38" width="21.0607287449393"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="38" width="49.2186234817814"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="38" width="34.6437246963563"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="38" width="10.4048582995951"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="39" width="10.4048582995951"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="39" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="37" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="37" width="20.6882591093117"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="37" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="37" width="51.5384615384615"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="37" width="36.3643724696356"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="37" width="10.6558704453441"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="38" width="10.6558704453441"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="38" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="32" t="s">
+      <c r="A1" s="39"/>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="39"/>
+      <c r="E1" s="39"/>
+      <c r="F1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="17" t="s">
@@ -2570,526 +2622,526 @@
         <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>69</v>
+        <v>39</v>
       </c>
       <c r="K2" s="18" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="M2" s="18" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="42" t="s">
-        <v>41</v>
+      <c r="B3" s="41" t="s">
+        <v>45</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>40</v>
-      </c>
-      <c r="F3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="44" t="n">
+        <v>43</v>
+      </c>
+      <c r="E3" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L3" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C4" s="23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="E4" s="21" t="n">
         <v>3582910032373</v>
       </c>
-      <c r="F4" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="44" t="n">
+      <c r="F4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="22" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C5" s="23" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="E5" s="21" t="n">
         <v>3582910034988</v>
       </c>
-      <c r="F5" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M5" s="44" t="n">
+      <c r="F5" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M5" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="22" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="43" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" s="44" t="n">
+        <v>50</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="22" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="E7" s="21" t="n">
         <v>201513619</v>
       </c>
-      <c r="F7" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="K7" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="L7" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="M7" s="44" t="n">
+      <c r="F7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="K7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="M7" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="41" t="s">
+      <c r="A8" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C8" s="22" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="45" t="s">
-        <v>53</v>
-      </c>
-      <c r="F8" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="L8" s="44" t="n">
-        <v>1</v>
-      </c>
-      <c r="M8" s="44" t="n">
+        <v>56</v>
+      </c>
+      <c r="E8" s="44" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="M8" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="22" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C9" s="22" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>59</v>
-      </c>
-      <c r="F9" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="44" t="n">
+        <v>62</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="F9" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="41" t="s">
+      <c r="A10" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="27" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C10" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F10" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L10" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M10" s="44" t="n">
+        <v>67</v>
+      </c>
+      <c r="F10" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K10" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L10" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M10" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="41" t="s">
+      <c r="A11" s="40" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="27" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="F11" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="L11" s="44" t="n">
-        <v>0</v>
-      </c>
-      <c r="M11" s="44" t="n">
+        <v>71</v>
+      </c>
+      <c r="F11" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="K11" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="L11" s="43" t="n">
+        <v>0</v>
+      </c>
+      <c r="M11" s="43" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H12" s="38"/>
-      <c r="I12" s="38"/>
+      <c r="H12" s="37"/>
+      <c r="I12" s="37"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
+      <c r="H13" s="37"/>
+      <c r="I13" s="37"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
+      <c r="H14" s="37"/>
+      <c r="I14" s="37"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
+      <c r="H15" s="37"/>
+      <c r="I15" s="37"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
+      <c r="H17" s="37"/>
+      <c r="I17" s="37"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
+      <c r="H18" s="37"/>
+      <c r="I18" s="37"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
+      <c r="H19" s="37"/>
+      <c r="I19" s="37"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
+      <c r="H20" s="37"/>
+      <c r="I20" s="37"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
+      <c r="H21" s="37"/>
+      <c r="I21" s="37"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
+      <c r="H22" s="37"/>
+      <c r="I22" s="37"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
+      <c r="H23" s="37"/>
+      <c r="I23" s="37"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
+      <c r="H24" s="37"/>
+      <c r="I24" s="37"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
+      <c r="H25" s="37"/>
+      <c r="I25" s="37"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="38"/>
-      <c r="I27" s="38"/>
+      <c r="H27" s="37"/>
+      <c r="I27" s="37"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="38"/>
-      <c r="I28" s="38"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="38"/>
-      <c r="I29" s="38"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
+      <c r="H30" s="37"/>
+      <c r="I30" s="37"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
+      <c r="H31" s="37"/>
+      <c r="I31" s="37"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="38"/>
-      <c r="I32" s="38"/>
+      <c r="H32" s="37"/>
+      <c r="I32" s="37"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="38"/>
-      <c r="I33" s="38"/>
+      <c r="H33" s="37"/>
+      <c r="I33" s="37"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="38"/>
-      <c r="I34" s="38"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="37"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="38"/>
-      <c r="I35" s="38"/>
+      <c r="H35" s="37"/>
+      <c r="I35" s="37"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="38"/>
-      <c r="I36" s="38"/>
+      <c r="H36" s="37"/>
+      <c r="I36" s="37"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="38"/>
-      <c r="I37" s="38"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="38"/>
-      <c r="I38" s="38"/>
+      <c r="H38" s="37"/>
+      <c r="I38" s="37"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="38"/>
-      <c r="I39" s="38"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="38"/>
-      <c r="I40" s="38"/>
+      <c r="H40" s="37"/>
+      <c r="I40" s="37"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="38"/>
-      <c r="I41" s="38"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="37"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="38"/>
-      <c r="I42" s="38"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="37"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="38"/>
-      <c r="I43" s="38"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="37"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="38"/>
-      <c r="I44" s="38"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="37"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="38"/>
-      <c r="I45" s="38"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="37"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="38"/>
-      <c r="I46" s="38"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3111,22 +3163,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:M2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="47" width="28.7732793522267"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="48" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="47" width="30.3562753036437"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="48" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="48" width="19.2186234817814"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="28" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="29" width="11.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="49" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="28" width="30.1133603238866"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="46" width="34.1578947368421"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="28" width="31.82995951417"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="46" width="27.9068825910931"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="46" width="20.1943319838057"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="28" width="11.6315789473684"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="29" width="11.6315789473684"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="47" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3135,27 +3187,31 @@
       <c r="C1" s="15"/>
       <c r="D1" s="15"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="32" t="s">
+      <c r="F1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="50" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="48" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="18" t="s">
@@ -3171,179 +3227,179 @@
         <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="50" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="50" t="s">
+        <v>74</v>
+      </c>
+      <c r="D3" s="50" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="50" t="s">
+        <v>59</v>
+      </c>
+      <c r="F3" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M3" s="52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="50" t="s">
+        <v>75</v>
+      </c>
+      <c r="C4" s="50" t="s">
+        <v>76</v>
+      </c>
+      <c r="D4" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L4" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="M4" s="52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" s="50" t="s">
+        <v>78</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="E5" s="50" t="s">
+        <v>53</v>
+      </c>
+      <c r="F5" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="52" t="n">
+        <v>0</v>
+      </c>
+      <c r="L5" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="49" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="53" t="s">
+        <v>79</v>
+      </c>
+      <c r="C6" s="50" t="s">
+        <v>80</v>
+      </c>
+      <c r="D6" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="E6" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="18" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="52" t="s">
-        <v>73</v>
-      </c>
-      <c r="C3" s="52" t="s">
-        <v>74</v>
-      </c>
-      <c r="D3" s="52" t="s">
-        <v>54</v>
-      </c>
-      <c r="E3" s="52" t="s">
-        <v>55</v>
-      </c>
-      <c r="F3" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M3" s="54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="52" t="s">
-        <v>75</v>
-      </c>
-      <c r="C4" s="52" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="L4" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="52" t="s">
-        <v>78</v>
-      </c>
-      <c r="D5" s="52" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="52" t="s">
-        <v>49</v>
-      </c>
-      <c r="F5" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="53" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="54" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="51" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="55" t="s">
-        <v>79</v>
-      </c>
-      <c r="C6" s="52" t="s">
-        <v>80</v>
-      </c>
-      <c r="D6" s="52" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="56" t="s">
-        <v>65</v>
-      </c>
-      <c r="F6" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G6" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="H6" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="53" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="54" t="n">
-        <v>1</v>
-      </c>
-      <c r="M6" s="54" t="n">
+      <c r="F6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="L6" s="52" t="n">
+        <v>1</v>
+      </c>
+      <c r="M6" s="52" t="n">
         <v>1</v>
       </c>
     </row>
@@ -3353,6 +3409,7 @@
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
@@ -3381,49 +3438,53 @@
   </sheetPr>
   <dimension ref="A1:M80"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J2" activeCellId="0" sqref="J2:M2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="57" width="31.4655870445344"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="57" width="43.2105263157895"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="57" width="19.0971659919028"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="57" width="17.6234817813765"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="57" width="16.6477732793522"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="58" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="59" width="9.54655870445344"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="60" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="55" width="33.0485829959514"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="55" width="45.417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="55" width="20.0728744939271"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="55" width="18.3684210526316"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="55" width="17.3805668016194"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="56" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="57" width="9.78947368421053"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="58" width="9.30364372469636"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="61"/>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="61"/>
-      <c r="F1" s="32" t="s">
+      <c r="A1" s="59"/>
+      <c r="B1" s="59"/>
+      <c r="C1" s="59"/>
+      <c r="D1" s="59"/>
+      <c r="E1" s="59"/>
+      <c r="F1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="62" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="62" t="s">
+      <c r="A2" s="60" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="48" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="18" t="s">
@@ -3439,847 +3500,847 @@
         <v>38</v>
       </c>
       <c r="J2" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="L2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="M2" s="18" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="62" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="63" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="64" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="L3" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="M3" s="66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="63" t="n">
+        <v>3582910032373</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="M4" s="66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="62" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" s="63" t="n">
+        <v>3582910034988</v>
+      </c>
+      <c r="D5" s="64" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" s="65" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="M5" s="66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="62" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="H6" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="M6" s="66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="62" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" s="63" t="n">
+        <v>201513619</v>
+      </c>
+      <c r="D7" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="G7" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="H7" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="K7" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="L7" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="M7" s="66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="62" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="F8" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="G8" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="H8" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="K8" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="L8" s="66" t="n">
+        <v>2</v>
+      </c>
+      <c r="M8" s="66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="62" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="D9" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="F9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="L9" s="66" t="n">
+        <v>0</v>
+      </c>
+      <c r="M9" s="66" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="62" t="s">
+        <v>62</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="D10" s="64" t="s">
+        <v>64</v>
+      </c>
+      <c r="E10" s="64" t="s">
+        <v>65</v>
+      </c>
+      <c r="F10" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="L10" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="M10" s="66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="62" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="64" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="18" t="s">
+      <c r="F11" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="L11" s="66" t="n">
+        <v>1</v>
+      </c>
+      <c r="M11" s="66" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="61" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="62" t="s">
         <v>70</v>
       </c>
-      <c r="L2" s="18" t="s">
+      <c r="C12" s="63" t="s">
         <v>71</v>
       </c>
-      <c r="M2" s="18" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="64" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" s="65" t="s">
-        <v>40</v>
-      </c>
-      <c r="D3" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="F3" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="L3" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="64" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="65" t="n">
-        <v>3582910032373</v>
-      </c>
-      <c r="D4" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="F4" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="K4" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="L4" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="M4" s="68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="64" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="65" t="n">
-        <v>3582910034988</v>
-      </c>
-      <c r="D5" s="66" t="s">
-        <v>44</v>
-      </c>
-      <c r="E5" s="67" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="K5" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="L5" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="M5" s="68" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="64" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="F6" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="G6" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="H6" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="K6" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="L6" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="M6" s="68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="64" t="s">
+      <c r="D12" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="E12" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="F12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="68" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="K12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" s="68" t="n">
+        <v>1</v>
+      </c>
+      <c r="M12" s="68" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" s="70" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="63" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="64" t="s">
+        <v>58</v>
+      </c>
+      <c r="E13" s="64" t="s">
+        <v>59</v>
+      </c>
+      <c r="F13" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="K13" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="L13" s="72" t="n">
+        <v>0</v>
+      </c>
+      <c r="M13" s="72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="70" t="s">
         <v>50</v>
       </c>
-      <c r="C7" s="65" t="n">
+      <c r="C14" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="71" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="71" t="n">
+        <v>0</v>
+      </c>
+      <c r="L14" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="M14" s="72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="70" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="63" t="n">
         <v>201513619</v>
       </c>
-      <c r="D7" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="E7" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="F7" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="G7" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="H7" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="K7" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="L7" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="M7" s="68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="64" t="s">
-        <v>52</v>
-      </c>
-      <c r="C8" s="65" t="s">
+      <c r="D15" s="64" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="64" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="F8" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="G8" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="H8" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="K8" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="L8" s="68" t="n">
-        <v>2</v>
-      </c>
-      <c r="M8" s="68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="64" t="s">
-        <v>56</v>
-      </c>
-      <c r="C9" s="65" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="F9" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="L9" s="68" t="n">
-        <v>0</v>
-      </c>
-      <c r="M9" s="68" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="C10" s="65" t="s">
-        <v>59</v>
-      </c>
-      <c r="D10" s="66" t="s">
-        <v>60</v>
-      </c>
-      <c r="E10" s="66" t="s">
-        <v>61</v>
-      </c>
-      <c r="F10" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="L10" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="M10" s="68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B11" s="64" t="s">
-        <v>62</v>
-      </c>
-      <c r="C11" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="D11" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="E11" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="F11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="L11" s="68" t="n">
-        <v>1</v>
-      </c>
-      <c r="M11" s="68" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="63" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="64" t="s">
+      <c r="F15" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="73" t="n">
+        <v>1</v>
+      </c>
+      <c r="K15" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="L15" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="M15" s="72" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="69" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="70" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="65" t="s">
+      <c r="C16" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="D12" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="E12" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="F12" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="70" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="K12" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="L12" s="70" t="n">
-        <v>1</v>
-      </c>
-      <c r="M12" s="70" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" s="72" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="65" t="s">
-        <v>53</v>
-      </c>
-      <c r="D13" s="66" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="F13" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="G13" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="H13" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="K13" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="L13" s="74" t="n">
-        <v>0</v>
-      </c>
-      <c r="M13" s="74" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="72" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="65" t="s">
-        <v>47</v>
-      </c>
-      <c r="D14" s="66" t="s">
-        <v>48</v>
-      </c>
-      <c r="E14" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="F14" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="73" t="n">
-        <v>1</v>
-      </c>
-      <c r="K14" s="73" t="n">
-        <v>0</v>
-      </c>
-      <c r="L14" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="M14" s="74" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="72" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="65" t="n">
-        <v>201513619</v>
-      </c>
-      <c r="D15" s="66" t="s">
-        <v>51</v>
-      </c>
-      <c r="E15" s="66" t="s">
-        <v>49</v>
-      </c>
-      <c r="F15" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="75" t="n">
-        <v>1</v>
-      </c>
-      <c r="K15" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="L15" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="M15" s="74" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="71" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="72" t="s">
-        <v>62</v>
-      </c>
-      <c r="C16" s="65" t="s">
-        <v>63</v>
-      </c>
-      <c r="D16" s="69" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="66" t="s">
-        <v>65</v>
-      </c>
-      <c r="F16" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="G16" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="H16" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="75" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="K16" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="L16" s="74" t="n">
-        <v>1</v>
-      </c>
-      <c r="M16" s="74" t="n">
+      <c r="D16" s="67" t="s">
+        <v>68</v>
+      </c>
+      <c r="E16" s="64" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="73" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="K16" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="L16" s="72" t="n">
+        <v>1</v>
+      </c>
+      <c r="M16" s="72" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="58"/>
-      <c r="I17" s="58"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="56"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="58"/>
-      <c r="I18" s="58"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="56"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="58"/>
-      <c r="I19" s="58"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="58"/>
-      <c r="I20" s="58"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="56"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="58"/>
-      <c r="I21" s="58"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="56"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="58"/>
-      <c r="I22" s="58"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="56"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="58"/>
-      <c r="I23" s="58"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="56"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="58"/>
-      <c r="I24" s="58"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="56"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="58"/>
-      <c r="I25" s="58"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="56"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="58"/>
-      <c r="I26" s="58"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="56"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="58"/>
-      <c r="I27" s="58"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="56"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="58"/>
-      <c r="I28" s="58"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="56"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="58"/>
-      <c r="I29" s="58"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="56"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="58"/>
-      <c r="I30" s="58"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="58"/>
-      <c r="I31" s="58"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="58"/>
-      <c r="I32" s="58"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="56"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="58"/>
-      <c r="I33" s="58"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="56"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="58"/>
-      <c r="I34" s="58"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="56"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="58"/>
-      <c r="I35" s="58"/>
+      <c r="H35" s="56"/>
+      <c r="I35" s="56"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="58"/>
-      <c r="I36" s="58"/>
+      <c r="H36" s="56"/>
+      <c r="I36" s="56"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="58"/>
-      <c r="I37" s="58"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="58"/>
-      <c r="I38" s="58"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="58"/>
-      <c r="I39" s="58"/>
+      <c r="H39" s="56"/>
+      <c r="I39" s="56"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="58"/>
-      <c r="I40" s="58"/>
+      <c r="H40" s="56"/>
+      <c r="I40" s="56"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="58"/>
-      <c r="I41" s="58"/>
+      <c r="H41" s="56"/>
+      <c r="I41" s="56"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="58"/>
-      <c r="I42" s="58"/>
+      <c r="H42" s="56"/>
+      <c r="I42" s="56"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="58"/>
-      <c r="I43" s="58"/>
+      <c r="H43" s="56"/>
+      <c r="I43" s="56"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="58"/>
-      <c r="I44" s="58"/>
+      <c r="H44" s="56"/>
+      <c r="I44" s="56"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="58"/>
-      <c r="I45" s="58"/>
+      <c r="H45" s="56"/>
+      <c r="I45" s="56"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="58"/>
-      <c r="I46" s="58"/>
+      <c r="H46" s="56"/>
+      <c r="I46" s="56"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="58"/>
-      <c r="I47" s="58"/>
+      <c r="H47" s="56"/>
+      <c r="I47" s="56"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="58"/>
-      <c r="I48" s="58"/>
+      <c r="H48" s="56"/>
+      <c r="I48" s="56"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H49" s="58"/>
-      <c r="I49" s="58"/>
+      <c r="H49" s="56"/>
+      <c r="I49" s="56"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
+      <c r="H50" s="56"/>
+      <c r="I50" s="56"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
+      <c r="H51" s="56"/>
+      <c r="I51" s="56"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
+      <c r="H52" s="56"/>
+      <c r="I52" s="56"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H53" s="58"/>
-      <c r="I53" s="58"/>
+      <c r="H53" s="56"/>
+      <c r="I53" s="56"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H54" s="58"/>
-      <c r="I54" s="58"/>
+      <c r="H54" s="56"/>
+      <c r="I54" s="56"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H55" s="58"/>
-      <c r="I55" s="58"/>
+      <c r="H55" s="56"/>
+      <c r="I55" s="56"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H56" s="58"/>
-      <c r="I56" s="58"/>
+      <c r="H56" s="56"/>
+      <c r="I56" s="56"/>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H57" s="58"/>
-      <c r="I57" s="58"/>
+      <c r="H57" s="56"/>
+      <c r="I57" s="56"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H58" s="58"/>
-      <c r="I58" s="58"/>
+      <c r="H58" s="56"/>
+      <c r="I58" s="56"/>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H59" s="58"/>
-      <c r="I59" s="58"/>
+      <c r="H59" s="56"/>
+      <c r="I59" s="56"/>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H60" s="58"/>
-      <c r="I60" s="58"/>
+      <c r="H60" s="56"/>
+      <c r="I60" s="56"/>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H61" s="58"/>
-      <c r="I61" s="58"/>
+      <c r="H61" s="56"/>
+      <c r="I61" s="56"/>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H62" s="58"/>
-      <c r="I62" s="58"/>
+      <c r="H62" s="56"/>
+      <c r="I62" s="56"/>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H63" s="58"/>
-      <c r="I63" s="58"/>
+      <c r="H63" s="56"/>
+      <c r="I63" s="56"/>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H64" s="58"/>
-      <c r="I64" s="58"/>
+      <c r="H64" s="56"/>
+      <c r="I64" s="56"/>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H65" s="58"/>
-      <c r="I65" s="58"/>
+      <c r="H65" s="56"/>
+      <c r="I65" s="56"/>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H66" s="58"/>
-      <c r="I66" s="58"/>
+      <c r="H66" s="56"/>
+      <c r="I66" s="56"/>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H67" s="58"/>
-      <c r="I67" s="58"/>
+      <c r="H67" s="56"/>
+      <c r="I67" s="56"/>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H68" s="58"/>
-      <c r="I68" s="58"/>
+      <c r="H68" s="56"/>
+      <c r="I68" s="56"/>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H69" s="58"/>
-      <c r="I69" s="58"/>
+      <c r="H69" s="56"/>
+      <c r="I69" s="56"/>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H70" s="58"/>
-      <c r="I70" s="58"/>
+      <c r="H70" s="56"/>
+      <c r="I70" s="56"/>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H71" s="58"/>
-      <c r="I71" s="58"/>
+      <c r="H71" s="56"/>
+      <c r="I71" s="56"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H72" s="58"/>
-      <c r="I72" s="58"/>
+      <c r="H72" s="56"/>
+      <c r="I72" s="56"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H73" s="58"/>
-      <c r="I73" s="58"/>
+      <c r="H73" s="56"/>
+      <c r="I73" s="56"/>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H74" s="58"/>
-      <c r="I74" s="58"/>
+      <c r="H74" s="56"/>
+      <c r="I74" s="56"/>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H75" s="58"/>
-      <c r="I75" s="58"/>
+      <c r="H75" s="56"/>
+      <c r="I75" s="56"/>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H76" s="58"/>
-      <c r="I76" s="58"/>
+      <c r="H76" s="56"/>
+      <c r="I76" s="56"/>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H77" s="58"/>
-      <c r="I77" s="58"/>
+      <c r="H77" s="56"/>
+      <c r="I77" s="56"/>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H78" s="58"/>
-      <c r="I78" s="58"/>
+      <c r="H78" s="56"/>
+      <c r="I78" s="56"/>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H79" s="58"/>
-      <c r="I79" s="58"/>
+      <c r="H79" s="56"/>
+      <c r="I79" s="56"/>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H80" s="58"/>
-      <c r="I80" s="58"/>
+      <c r="H80" s="56"/>
+      <c r="I80" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
adding the amended templ
</commit_message>
<xml_diff>
--- a/Projects/SANOFISA/Data/Template.xlsx
+++ b/Projects/SANOFISA/Data/Template.xlsx
@@ -888,13 +888,13 @@
     <t xml:space="preserve">CCDUAL_SECOND_18_001</t>
   </si>
   <si>
+    <t xml:space="preserve">COUGH</t>
+  </si>
+  <si>
     <t xml:space="preserve">TELFAST SECONDARY</t>
   </si>
   <si>
     <t xml:space="preserve">TEL_SECOND_18_001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cough &amp; Cold</t>
   </si>
 </sst>
 </file>
@@ -1244,7 +1244,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="83">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1393,10 +1393,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="166" fontId="18" fillId="6" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1467,10 +1463,6 @@
     </xf>
     <xf numFmtId="167" fontId="13" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1666,18 +1658,18 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.7449392712551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.1052631578947"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.2105263157895"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -1943,14 +1935,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="48.9514170040486"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="21.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.7813765182186"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="17.1376518218624"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="49.3805668016194"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.0647773279352"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.8906882591093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="17.246963562753"/>
     <col collapsed="false" hidden="false" max="9" min="6" style="13" width="11.6761133603239"/>
     <col collapsed="false" hidden="false" max="11" min="10" style="14" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="15" width="21.7449392712551"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="15" width="21.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="15" width="8.89068825910931"/>
   </cols>
   <sheetData>
@@ -2376,21 +2368,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="24.8502024291498"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="35" width="21.1012145748988"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="30.7449392712551"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="21.1012145748988"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="35" width="21.2105263157895"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="31.0647773279352"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="21.2105263157895"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="35" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="36" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="37" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="8.89068825910931"/>
   </cols>
   <sheetData>
-    <row r="1" s="15" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="38"/>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
       <c r="F1" s="17" t="s">
         <v>30</v>
       </c>
@@ -2431,10 +2423,10 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="40"/>
       <c r="E3" s="13"/>
       <c r="F3" s="28"/>
       <c r="G3" s="28"/>
@@ -2442,30 +2434,30 @@
       <c r="I3" s="28"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="39"/>
-      <c r="B4" s="42"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="43"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
       <c r="H4" s="28"/>
       <c r="I4" s="28"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="39"/>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="43"/>
+      <c r="A5" s="38"/>
+      <c r="B5" s="41"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
       <c r="F5" s="28"/>
       <c r="G5" s="28"/>
       <c r="H5" s="28"/>
       <c r="I5" s="28"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39"/>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="43"/>
+      <c r="A6" s="38"/>
+      <c r="B6" s="41"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
       <c r="F6" s="28"/>
       <c r="G6" s="28"/>
       <c r="H6" s="28"/>
@@ -2499,22 +2491,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="44" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="19.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="45" width="20.6720647773279"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="48.417004048583"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="34.17004048583"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="44" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="46" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="46" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="43" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="19.6032388663968"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="20.7813765182186"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="48.8461538461539"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="34.4939271255061"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="43" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="45" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="45" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="47"/>
-      <c r="B1" s="47"/>
-      <c r="C1" s="47"/>
-      <c r="D1" s="47"/>
-      <c r="E1" s="47"/>
+      <c r="A1" s="46"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
       <c r="F1" s="17" t="s">
         <v>30</v>
       </c>
@@ -2556,45 +2548,45 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="47" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="49" t="s">
+      <c r="B3" s="48" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="50" t="s">
+      <c r="C3" s="49" t="s">
         <v>43</v>
       </c>
       <c r="D3" s="24" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="51" t="s">
+      <c r="E3" s="50" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="52" t="n">
+      <c r="F3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="48" t="s">
+      <c r="A4" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B4" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="50" t="s">
+      <c r="C4" s="49" t="s">
         <v>43</v>
       </c>
       <c r="D4" s="24" t="s">
@@ -2603,30 +2595,30 @@
       <c r="E4" s="25" t="n">
         <v>3582910032373</v>
       </c>
-      <c r="F4" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="52" t="n">
+      <c r="F4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="48" t="s">
+      <c r="A5" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B5" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="C5" s="49" t="s">
         <v>43</v>
       </c>
       <c r="D5" s="24" t="s">
@@ -2635,62 +2627,62 @@
       <c r="E5" s="25" t="n">
         <v>3582910034988</v>
       </c>
-      <c r="F5" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G5" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I5" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="52" t="n">
+      <c r="F5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="48" t="s">
+      <c r="A6" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B6" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C6" s="53" t="s">
+      <c r="C6" s="52" t="s">
         <v>50</v>
       </c>
       <c r="D6" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="E6" s="51" t="s">
+      <c r="E6" s="50" t="s">
         <v>48</v>
       </c>
-      <c r="F6" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="52" t="n">
+      <c r="F6" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="48" t="s">
+      <c r="A7" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="53" t="s">
+      <c r="C7" s="52" t="s">
         <v>50</v>
       </c>
       <c r="D7" s="24" t="s">
@@ -2699,62 +2691,62 @@
       <c r="E7" s="25" t="n">
         <v>201513619</v>
       </c>
-      <c r="F7" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="52" t="n">
+      <c r="F7" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J7" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="48" t="s">
+      <c r="A8" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="53" t="s">
+      <c r="C8" s="52" t="s">
         <v>56</v>
       </c>
       <c r="D8" s="24" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="54" t="s">
+      <c r="E8" s="53" t="s">
         <v>54</v>
       </c>
-      <c r="F8" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="52" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J8" s="52" t="n">
+      <c r="F8" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J8" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="48" t="s">
+      <c r="A9" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B9" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="C9" s="53" t="s">
+      <c r="C9" s="52" t="s">
         <v>56</v>
       </c>
       <c r="D9" s="24" t="s">
@@ -2763,62 +2755,62 @@
       <c r="E9" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="F9" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G9" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H9" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I9" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="52" t="n">
+      <c r="F9" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H9" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="48" t="s">
+      <c r="A10" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C10" s="53" t="s">
+      <c r="C10" s="52" t="s">
         <v>62</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="55" t="s">
+      <c r="E10" s="54" t="s">
         <v>60</v>
       </c>
-      <c r="F10" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G10" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H10" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I10" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J10" s="52" t="n">
+      <c r="F10" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H10" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I10" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J10" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="48" t="s">
+      <c r="A11" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="53" t="s">
+      <c r="C11" s="52" t="s">
         <v>66</v>
       </c>
       <c r="D11" s="24" t="s">
@@ -2827,30 +2819,30 @@
       <c r="E11" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="F11" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G11" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H11" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I11" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J11" s="52" t="n">
+      <c r="F11" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H11" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J11" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="48" t="s">
+      <c r="A12" s="47" t="s">
         <v>14</v>
       </c>
       <c r="B12" s="32" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="53" t="s">
+      <c r="C12" s="52" t="s">
         <v>66</v>
       </c>
       <c r="D12" s="24" t="s">
@@ -2859,196 +2851,196 @@
       <c r="E12" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G12" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="H12" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="I12" s="52" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="52" t="n">
+      <c r="F12" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" s="51" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="51" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="44"/>
-      <c r="I14" s="44"/>
-      <c r="J14" s="44"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="44"/>
-      <c r="I15" s="44"/>
-      <c r="J15" s="44"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="44"/>
-      <c r="I16" s="44"/>
-      <c r="J16" s="44"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="44"/>
-      <c r="I17" s="44"/>
-      <c r="J17" s="44"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="44"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="44"/>
-      <c r="I21" s="44"/>
-      <c r="J21" s="44"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="44"/>
-      <c r="I22" s="44"/>
-      <c r="J22" s="44"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="44"/>
-      <c r="I26" s="44"/>
-      <c r="J26" s="44"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="44"/>
-      <c r="I27" s="44"/>
-      <c r="J27" s="44"/>
+      <c r="H27" s="43"/>
+      <c r="I27" s="43"/>
+      <c r="J27" s="43"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="44"/>
-      <c r="I28" s="44"/>
-      <c r="J28" s="44"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="H30" s="43"/>
+      <c r="I30" s="43"/>
+      <c r="J30" s="43"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="44"/>
-      <c r="I31" s="44"/>
-      <c r="J31" s="44"/>
+      <c r="H31" s="43"/>
+      <c r="I31" s="43"/>
+      <c r="J31" s="43"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
-      <c r="J32" s="44"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="44"/>
-      <c r="I33" s="44"/>
-      <c r="J33" s="44"/>
+      <c r="H33" s="43"/>
+      <c r="I33" s="43"/>
+      <c r="J33" s="43"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="44"/>
+      <c r="H34" s="43"/>
+      <c r="I34" s="43"/>
+      <c r="J34" s="43"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="44"/>
-      <c r="I35" s="44"/>
-      <c r="J35" s="44"/>
+      <c r="H35" s="43"/>
+      <c r="I35" s="43"/>
+      <c r="J35" s="43"/>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="44"/>
-      <c r="I36" s="44"/>
-      <c r="J36" s="44"/>
+      <c r="H36" s="43"/>
+      <c r="I36" s="43"/>
+      <c r="J36" s="43"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="44"/>
-      <c r="I37" s="44"/>
-      <c r="J37" s="44"/>
+      <c r="H37" s="43"/>
+      <c r="I37" s="43"/>
+      <c r="J37" s="43"/>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="44"/>
-      <c r="I38" s="44"/>
-      <c r="J38" s="44"/>
+      <c r="H38" s="43"/>
+      <c r="I38" s="43"/>
+      <c r="J38" s="43"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="44"/>
-      <c r="I39" s="44"/>
-      <c r="J39" s="44"/>
+      <c r="H39" s="43"/>
+      <c r="I39" s="43"/>
+      <c r="J39" s="43"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="43"/>
+      <c r="J40" s="43"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="44"/>
-      <c r="I41" s="44"/>
-      <c r="J41" s="44"/>
+      <c r="H41" s="43"/>
+      <c r="I41" s="43"/>
+      <c r="J41" s="43"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="44"/>
-      <c r="I42" s="44"/>
-      <c r="J42" s="44"/>
+      <c r="H42" s="43"/>
+      <c r="I42" s="43"/>
+      <c r="J42" s="43"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="44"/>
-      <c r="I43" s="44"/>
-      <c r="J43" s="44"/>
+      <c r="H43" s="43"/>
+      <c r="I43" s="43"/>
+      <c r="J43" s="43"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="44"/>
-      <c r="I44" s="44"/>
-      <c r="J44" s="44"/>
+      <c r="H44" s="43"/>
+      <c r="I44" s="43"/>
+      <c r="J44" s="43"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="44"/>
-      <c r="I45" s="44"/>
-      <c r="J45" s="44"/>
+      <c r="H45" s="43"/>
+      <c r="I45" s="43"/>
+      <c r="J45" s="43"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="44"/>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="H46" s="43"/>
+      <c r="I46" s="43"/>
+      <c r="J46" s="43"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="44"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="43"/>
+      <c r="J47" s="43"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3073,19 +3065,19 @@
   <dimension ref="A1:J7"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
+      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="56" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="57" width="32.1376518218623"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="56" width="29.7773279352227"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="57" width="26.1376518218623"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="57" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="55" width="32.3481781376518"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="35" width="29.9919028340081"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="55" width="26.3522267206478"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="55" width="18.8542510121457"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="35" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="9" min="8" style="36" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="58" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="56" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3103,19 +3095,19 @@
       <c r="J1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="59" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="59" t="s">
+      <c r="A2" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="59" t="s">
+      <c r="C2" s="57" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="57" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="20" t="s">
@@ -3135,130 +3127,130 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="60" t="s">
+      <c r="A3" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B3" s="61" t="s">
+      <c r="B3" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="C3" s="61" t="s">
+      <c r="C3" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="61" t="s">
+      <c r="E3" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G3" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="H3" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="I3" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J3" s="63" t="n">
+      <c r="F3" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H3" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I3" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J3" s="61" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="60" t="s">
+      <c r="A4" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="61" t="s">
+      <c r="B4" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="C4" s="61" t="s">
+      <c r="C4" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="61" t="s">
+      <c r="E4" s="59" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="G4" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="H4" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="I4" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J4" s="63" t="n">
+      <c r="F4" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J4" s="61" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="60" t="s">
+      <c r="A5" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="62" t="s">
         <v>74</v>
       </c>
-      <c r="C5" s="61" t="s">
+      <c r="C5" s="59" t="s">
         <v>75</v>
       </c>
-      <c r="D5" s="61" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" s="61" t="s">
+      <c r="D5" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="E5" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="F5" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="H5" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="63" t="n">
+      <c r="F5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="H5" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="61" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="60" t="s">
+      <c r="A6" s="58" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="64" t="s">
-        <v>76</v>
-      </c>
-      <c r="C6" s="61" t="s">
+      <c r="B6" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="C6" s="59" t="s">
+        <v>78</v>
+      </c>
+      <c r="D6" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="65" t="s">
+      <c r="E6" s="63" t="s">
         <v>66</v>
       </c>
-      <c r="F6" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="62" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="I6" s="62" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="63" t="n">
+      <c r="F6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="60" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" s="60" t="n">
+        <v>0</v>
+      </c>
+      <c r="J6" s="61" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3297,28 +3289,28 @@
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C23" activeCellId="0" sqref="C23"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="66" width="30.8502024291498"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="66" width="42.6315789473684"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="67" width="18.6396761133603"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="67" width="17.4615384615385"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="67" width="27.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="67" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="68" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="68" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="69" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="64" width="31.17004048583"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="64" width="43.0607287449393"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="65" width="18.7449392712551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="65" width="17.5668016194332"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="65" width="27.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="65" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="66" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="66" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="67" width="8.89068825910931"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="70"/>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
-      <c r="E1" s="70"/>
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
       <c r="F1" s="17" t="s">
         <v>30</v>
       </c>
@@ -3328,19 +3320,19 @@
       <c r="J1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="71" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="71" t="s">
+      <c r="A2" s="69" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="69" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="71" t="s">
+      <c r="C2" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="59" t="s">
+      <c r="D2" s="57" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="59" t="s">
+      <c r="E2" s="57" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="20" t="s">
@@ -3360,762 +3352,762 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="72" t="s">
+      <c r="A3" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="73" t="s">
+      <c r="B3" s="71" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="72" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="73" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="76" t="s">
+      <c r="E3" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="77" t="n">
+      <c r="F3" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="75" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="72" t="s">
+      <c r="A4" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="71" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="74" t="n">
+      <c r="C4" s="72" t="n">
         <v>3582910032373</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="76" t="s">
+      <c r="E4" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="77" t="n">
+      <c r="F4" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="75" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="74" t="n">
+      <c r="C5" s="72" t="n">
         <v>3582910034988</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="73" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="76" t="s">
+      <c r="E5" s="74" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="77" t="n">
+      <c r="F5" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="75" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="71" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="F6" s="77" t="n">
+      <c r="E6" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="G6" s="77" t="n">
+      <c r="G6" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="H6" s="77" t="n">
+      <c r="H6" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="I6" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="77" t="n">
+      <c r="I6" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="75" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="74" t="n">
+      <c r="C7" s="72" t="n">
         <v>201513619</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="77" t="n">
+      <c r="E7" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="G7" s="77" t="n">
+      <c r="G7" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="H7" s="77" t="n">
+      <c r="H7" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="I7" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="77" t="n">
+      <c r="I7" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="75" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="72" t="s">
+      <c r="A8" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="73" t="s">
+      <c r="B8" s="71" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="74" t="s">
+      <c r="C8" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="75" t="s">
+      <c r="D8" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="76" t="s">
+      <c r="E8" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="77" t="n">
+      <c r="F8" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="G8" s="77" t="n">
+      <c r="G8" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="H8" s="77" t="n">
+      <c r="H8" s="75" t="n">
         <v>2</v>
       </c>
-      <c r="I8" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="77" t="n">
+      <c r="I8" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="75" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="72" t="s">
+      <c r="A9" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="74" t="s">
+      <c r="C9" s="72" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="75" t="s">
+      <c r="D9" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="76" t="s">
+      <c r="E9" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="77" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="77" t="n">
+      <c r="F9" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="75" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="75" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="72" t="s">
+      <c r="A10" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="73" t="s">
+      <c r="B10" s="71" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="74" t="s">
+      <c r="C10" s="72" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="75" t="s">
+      <c r="D10" s="73" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="75" t="s">
+      <c r="E10" s="73" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="77" t="n">
+      <c r="F10" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="75" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="72" t="s">
+      <c r="A11" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="71" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="78" t="s">
+      <c r="D11" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="75" t="s">
+      <c r="E11" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="77" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="77" t="n">
+      <c r="F11" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="75" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="75" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="72" t="s">
+      <c r="A12" s="70" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="73" t="s">
+      <c r="B12" s="71" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="74" t="s">
+      <c r="C12" s="72" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="78" t="s">
+      <c r="D12" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="75" t="s">
+      <c r="E12" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="79" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="79" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="79" t="n">
+      <c r="F12" s="77" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="77" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="77" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="77" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="77" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B13" s="81" t="s">
+      <c r="B13" s="79" t="s">
         <v>53</v>
       </c>
-      <c r="C13" s="74" t="s">
+      <c r="C13" s="72" t="s">
         <v>54</v>
       </c>
-      <c r="D13" s="75" t="s">
+      <c r="D13" s="73" t="s">
         <v>55</v>
       </c>
-      <c r="E13" s="76" t="s">
+      <c r="E13" s="74" t="s">
         <v>56</v>
       </c>
-      <c r="F13" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="G13" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="H13" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="I13" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="J13" s="82" t="n">
+      <c r="F13" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H13" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="I13" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J13" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="80" t="s">
+      <c r="A14" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="81" t="s">
+      <c r="B14" s="79" t="s">
         <v>47</v>
       </c>
-      <c r="C14" s="74" t="s">
+      <c r="C14" s="72" t="s">
         <v>48</v>
       </c>
-      <c r="D14" s="75" t="s">
+      <c r="D14" s="73" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="F14" s="82" t="n">
-        <v>1</v>
-      </c>
-      <c r="G14" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="H14" s="82" t="n">
-        <v>1</v>
-      </c>
-      <c r="I14" s="82" t="n">
-        <v>0</v>
-      </c>
-      <c r="J14" s="82" t="n">
+      <c r="E14" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="H14" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="I14" s="80" t="n">
+        <v>0</v>
+      </c>
+      <c r="J14" s="80" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="80" t="s">
+      <c r="A15" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="81" t="s">
+      <c r="B15" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="74" t="n">
+      <c r="C15" s="72" t="n">
         <v>201513619</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="73" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="75" t="s">
-        <v>78</v>
-      </c>
-      <c r="F15" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="G15" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="H15" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="I15" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="J15" s="83" t="n">
+      <c r="E15" s="73" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="81" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" s="81" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J15" s="81" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="80" t="s">
+      <c r="A16" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="81" t="s">
+      <c r="B16" s="79" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="D16" s="78" t="s">
+      <c r="D16" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="E16" s="75" t="s">
+      <c r="E16" s="73" t="s">
         <v>66</v>
       </c>
-      <c r="F16" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="G16" s="83" t="n">
-        <v>1</v>
-      </c>
-      <c r="H16" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="83" t="n">
-        <v>0</v>
-      </c>
-      <c r="J16" s="84" t="n">
+      <c r="F16" s="81" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" s="81" t="n">
+        <v>1</v>
+      </c>
+      <c r="H16" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="81" t="n">
+        <v>0</v>
+      </c>
+      <c r="J16" s="82" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="67"/>
-      <c r="I17" s="67"/>
-      <c r="J17" s="67"/>
+      <c r="H17" s="65"/>
+      <c r="I17" s="65"/>
+      <c r="J17" s="65"/>
     </row>
     <row r="18" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
+      <c r="H18" s="65"/>
+      <c r="I18" s="65"/>
+      <c r="J18" s="65"/>
     </row>
     <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
+      <c r="H19" s="65"/>
+      <c r="I19" s="65"/>
+      <c r="J19" s="65"/>
     </row>
     <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
+      <c r="H20" s="65"/>
+      <c r="I20" s="65"/>
+      <c r="J20" s="65"/>
     </row>
     <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="65"/>
+      <c r="J21" s="65"/>
     </row>
     <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
+      <c r="H22" s="65"/>
+      <c r="I22" s="65"/>
+      <c r="J22" s="65"/>
     </row>
     <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
+      <c r="H23" s="65"/>
+      <c r="I23" s="65"/>
+      <c r="J23" s="65"/>
     </row>
     <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
+      <c r="H24" s="65"/>
+      <c r="I24" s="65"/>
+      <c r="J24" s="65"/>
     </row>
     <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
+      <c r="H25" s="65"/>
+      <c r="I25" s="65"/>
+      <c r="J25" s="65"/>
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
+      <c r="H26" s="65"/>
+      <c r="I26" s="65"/>
+      <c r="J26" s="65"/>
     </row>
     <row r="27" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="67"/>
-      <c r="I27" s="67"/>
-      <c r="J27" s="67"/>
+      <c r="H27" s="65"/>
+      <c r="I27" s="65"/>
+      <c r="J27" s="65"/>
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="67"/>
-      <c r="I28" s="67"/>
-      <c r="J28" s="67"/>
+      <c r="H28" s="65"/>
+      <c r="I28" s="65"/>
+      <c r="J28" s="65"/>
     </row>
     <row r="29" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="67"/>
-      <c r="I29" s="67"/>
-      <c r="J29" s="67"/>
+      <c r="H29" s="65"/>
+      <c r="I29" s="65"/>
+      <c r="J29" s="65"/>
     </row>
     <row r="30" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="67"/>
-      <c r="I30" s="67"/>
-      <c r="J30" s="67"/>
+      <c r="H30" s="65"/>
+      <c r="I30" s="65"/>
+      <c r="J30" s="65"/>
     </row>
     <row r="31" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="67"/>
-      <c r="I31" s="67"/>
-      <c r="J31" s="67"/>
+      <c r="H31" s="65"/>
+      <c r="I31" s="65"/>
+      <c r="J31" s="65"/>
     </row>
     <row r="32" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="67"/>
-      <c r="I32" s="67"/>
-      <c r="J32" s="67"/>
+      <c r="H32" s="65"/>
+      <c r="I32" s="65"/>
+      <c r="J32" s="65"/>
     </row>
     <row r="33" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="67"/>
-      <c r="I33" s="67"/>
-      <c r="J33" s="67"/>
+      <c r="H33" s="65"/>
+      <c r="I33" s="65"/>
+      <c r="J33" s="65"/>
     </row>
     <row r="34" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
     </row>
     <row r="35" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="67"/>
-      <c r="I35" s="67"/>
-      <c r="J35" s="67"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="65"/>
+      <c r="J35" s="65"/>
     </row>
     <row r="36" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="67"/>
-      <c r="I36" s="67"/>
-      <c r="J36" s="67"/>
+      <c r="H36" s="65"/>
+      <c r="I36" s="65"/>
+      <c r="J36" s="65"/>
     </row>
     <row r="37" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="67"/>
-      <c r="I37" s="67"/>
-      <c r="J37" s="67"/>
+      <c r="H37" s="65"/>
+      <c r="I37" s="65"/>
+      <c r="J37" s="65"/>
     </row>
     <row r="38" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H38" s="67"/>
-      <c r="I38" s="67"/>
-      <c r="J38" s="67"/>
+      <c r="H38" s="65"/>
+      <c r="I38" s="65"/>
+      <c r="J38" s="65"/>
     </row>
     <row r="39" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H39" s="67"/>
-      <c r="I39" s="67"/>
-      <c r="J39" s="67"/>
+      <c r="H39" s="65"/>
+      <c r="I39" s="65"/>
+      <c r="J39" s="65"/>
     </row>
     <row r="40" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="67"/>
+      <c r="H40" s="65"/>
+      <c r="I40" s="65"/>
+      <c r="J40" s="65"/>
     </row>
     <row r="41" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H41" s="67"/>
-      <c r="I41" s="67"/>
-      <c r="J41" s="67"/>
+      <c r="H41" s="65"/>
+      <c r="I41" s="65"/>
+      <c r="J41" s="65"/>
     </row>
     <row r="42" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H42" s="67"/>
-      <c r="I42" s="67"/>
-      <c r="J42" s="67"/>
+      <c r="H42" s="65"/>
+      <c r="I42" s="65"/>
+      <c r="J42" s="65"/>
     </row>
     <row r="43" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H43" s="67"/>
-      <c r="I43" s="67"/>
-      <c r="J43" s="67"/>
+      <c r="H43" s="65"/>
+      <c r="I43" s="65"/>
+      <c r="J43" s="65"/>
     </row>
     <row r="44" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H44" s="67"/>
-      <c r="I44" s="67"/>
-      <c r="J44" s="67"/>
+      <c r="H44" s="65"/>
+      <c r="I44" s="65"/>
+      <c r="J44" s="65"/>
     </row>
     <row r="45" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H45" s="67"/>
-      <c r="I45" s="67"/>
-      <c r="J45" s="67"/>
+      <c r="H45" s="65"/>
+      <c r="I45" s="65"/>
+      <c r="J45" s="65"/>
     </row>
     <row r="46" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H46" s="67"/>
-      <c r="I46" s="67"/>
-      <c r="J46" s="67"/>
+      <c r="H46" s="65"/>
+      <c r="I46" s="65"/>
+      <c r="J46" s="65"/>
     </row>
     <row r="47" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H47" s="67"/>
-      <c r="I47" s="67"/>
-      <c r="J47" s="67"/>
+      <c r="H47" s="65"/>
+      <c r="I47" s="65"/>
+      <c r="J47" s="65"/>
     </row>
     <row r="48" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H48" s="67"/>
-      <c r="I48" s="67"/>
-      <c r="J48" s="67"/>
+      <c r="H48" s="65"/>
+      <c r="I48" s="65"/>
+      <c r="J48" s="65"/>
     </row>
     <row r="49" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H49" s="67"/>
-      <c r="I49" s="67"/>
-      <c r="J49" s="67"/>
+      <c r="H49" s="65"/>
+      <c r="I49" s="65"/>
+      <c r="J49" s="65"/>
     </row>
     <row r="50" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H50" s="67"/>
-      <c r="I50" s="67"/>
-      <c r="J50" s="67"/>
+      <c r="H50" s="65"/>
+      <c r="I50" s="65"/>
+      <c r="J50" s="65"/>
     </row>
     <row r="51" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H51" s="67"/>
-      <c r="I51" s="67"/>
-      <c r="J51" s="67"/>
+      <c r="H51" s="65"/>
+      <c r="I51" s="65"/>
+      <c r="J51" s="65"/>
     </row>
     <row r="52" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H52" s="67"/>
-      <c r="I52" s="67"/>
-      <c r="J52" s="67"/>
+      <c r="H52" s="65"/>
+      <c r="I52" s="65"/>
+      <c r="J52" s="65"/>
     </row>
     <row r="53" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H53" s="67"/>
-      <c r="I53" s="67"/>
-      <c r="J53" s="67"/>
+      <c r="H53" s="65"/>
+      <c r="I53" s="65"/>
+      <c r="J53" s="65"/>
     </row>
     <row r="54" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H54" s="67"/>
-      <c r="I54" s="67"/>
-      <c r="J54" s="67"/>
+      <c r="H54" s="65"/>
+      <c r="I54" s="65"/>
+      <c r="J54" s="65"/>
     </row>
     <row r="55" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H55" s="67"/>
-      <c r="I55" s="67"/>
-      <c r="J55" s="67"/>
+      <c r="H55" s="65"/>
+      <c r="I55" s="65"/>
+      <c r="J55" s="65"/>
     </row>
     <row r="56" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H56" s="67"/>
-      <c r="I56" s="67"/>
-      <c r="J56" s="67"/>
+      <c r="H56" s="65"/>
+      <c r="I56" s="65"/>
+      <c r="J56" s="65"/>
     </row>
     <row r="57" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H57" s="67"/>
-      <c r="I57" s="67"/>
-      <c r="J57" s="67"/>
+      <c r="H57" s="65"/>
+      <c r="I57" s="65"/>
+      <c r="J57" s="65"/>
     </row>
     <row r="58" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H58" s="67"/>
-      <c r="I58" s="67"/>
-      <c r="J58" s="67"/>
+      <c r="H58" s="65"/>
+      <c r="I58" s="65"/>
+      <c r="J58" s="65"/>
     </row>
     <row r="59" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H59" s="67"/>
-      <c r="I59" s="67"/>
-      <c r="J59" s="67"/>
+      <c r="H59" s="65"/>
+      <c r="I59" s="65"/>
+      <c r="J59" s="65"/>
     </row>
     <row r="60" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H60" s="67"/>
-      <c r="I60" s="67"/>
-      <c r="J60" s="67"/>
+      <c r="H60" s="65"/>
+      <c r="I60" s="65"/>
+      <c r="J60" s="65"/>
     </row>
     <row r="61" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H61" s="67"/>
-      <c r="I61" s="67"/>
-      <c r="J61" s="67"/>
+      <c r="H61" s="65"/>
+      <c r="I61" s="65"/>
+      <c r="J61" s="65"/>
     </row>
     <row r="62" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H62" s="67"/>
-      <c r="I62" s="67"/>
-      <c r="J62" s="67"/>
+      <c r="H62" s="65"/>
+      <c r="I62" s="65"/>
+      <c r="J62" s="65"/>
     </row>
     <row r="63" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H63" s="67"/>
-      <c r="I63" s="67"/>
-      <c r="J63" s="67"/>
+      <c r="H63" s="65"/>
+      <c r="I63" s="65"/>
+      <c r="J63" s="65"/>
     </row>
     <row r="64" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H64" s="67"/>
-      <c r="I64" s="67"/>
-      <c r="J64" s="67"/>
+      <c r="H64" s="65"/>
+      <c r="I64" s="65"/>
+      <c r="J64" s="65"/>
     </row>
     <row r="65" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H65" s="67"/>
-      <c r="I65" s="67"/>
-      <c r="J65" s="67"/>
+      <c r="H65" s="65"/>
+      <c r="I65" s="65"/>
+      <c r="J65" s="65"/>
     </row>
     <row r="66" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H66" s="67"/>
-      <c r="I66" s="67"/>
-      <c r="J66" s="67"/>
+      <c r="H66" s="65"/>
+      <c r="I66" s="65"/>
+      <c r="J66" s="65"/>
     </row>
     <row r="67" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H67" s="67"/>
-      <c r="I67" s="67"/>
-      <c r="J67" s="67"/>
+      <c r="H67" s="65"/>
+      <c r="I67" s="65"/>
+      <c r="J67" s="65"/>
     </row>
     <row r="68" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H68" s="67"/>
-      <c r="I68" s="67"/>
-      <c r="J68" s="67"/>
+      <c r="H68" s="65"/>
+      <c r="I68" s="65"/>
+      <c r="J68" s="65"/>
     </row>
     <row r="69" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H69" s="67"/>
-      <c r="I69" s="67"/>
-      <c r="J69" s="67"/>
+      <c r="H69" s="65"/>
+      <c r="I69" s="65"/>
+      <c r="J69" s="65"/>
     </row>
     <row r="70" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H70" s="67"/>
-      <c r="I70" s="67"/>
-      <c r="J70" s="67"/>
+      <c r="H70" s="65"/>
+      <c r="I70" s="65"/>
+      <c r="J70" s="65"/>
     </row>
     <row r="71" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H71" s="67"/>
-      <c r="I71" s="67"/>
+      <c r="H71" s="65"/>
+      <c r="I71" s="65"/>
     </row>
     <row r="72" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H72" s="67"/>
-      <c r="I72" s="67"/>
+      <c r="H72" s="65"/>
+      <c r="I72" s="65"/>
     </row>
     <row r="73" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H73" s="67"/>
-      <c r="I73" s="67"/>
+      <c r="H73" s="65"/>
+      <c r="I73" s="65"/>
     </row>
     <row r="74" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H74" s="67"/>
-      <c r="I74" s="67"/>
+      <c r="H74" s="65"/>
+      <c r="I74" s="65"/>
     </row>
     <row r="75" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H75" s="67"/>
-      <c r="I75" s="67"/>
+      <c r="H75" s="65"/>
+      <c r="I75" s="65"/>
     </row>
     <row r="76" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H76" s="67"/>
-      <c r="I76" s="67"/>
+      <c r="H76" s="65"/>
+      <c r="I76" s="65"/>
     </row>
     <row r="77" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H77" s="67"/>
-      <c r="I77" s="67"/>
+      <c r="H77" s="65"/>
+      <c r="I77" s="65"/>
     </row>
     <row r="78" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H78" s="67"/>
-      <c r="I78" s="67"/>
+      <c r="H78" s="65"/>
+      <c r="I78" s="65"/>
     </row>
     <row r="79" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H79" s="67"/>
-      <c r="I79" s="67"/>
+      <c r="H79" s="65"/>
+      <c r="I79" s="65"/>
     </row>
     <row r="80" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H80" s="67"/>
-      <c r="I80" s="67"/>
+      <c r="H80" s="65"/>
+      <c r="I80" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
sanofiSA and sanofiTR update
</commit_message>
<xml_diff>
--- a/Projects/SANOFISA/Data/Template.xlsx
+++ b/Projects/SANOFISA/Data/Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIs" sheetId="1" state="visible" r:id="rId2"/>
@@ -1158,7 +1158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1171,6 +1171,13 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1288,6 +1295,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1300,7 +1311,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1316,7 +1331,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1348,15 +1363,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="13" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1364,11 +1379,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1384,24 +1395,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -1424,11 +1419,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="19" fillId="8" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="8" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1444,7 +1451,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="9" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="9" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1512,7 +1519,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="10" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="10" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1618,14 +1625,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.7125506072874"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.9595141700405"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.57085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.7651821862348"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="26.080971659919"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="19.4655870445344"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="19.82995951417"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.668016194332"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.0769230769231"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="25.587044534413"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.81376518218623"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1885,415 +1892,415 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="0" topLeftCell="C1" activePane="topRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="topRight" activeCell="C24" activeCellId="0" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="49.7044534412956"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.2793522267206"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="17.995951417004"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="17.3522267206478"/>
-    <col collapsed="false" hidden="false" max="9" min="6" style="13" width="11.6761133603239"/>
-    <col collapsed="false" hidden="false" max="11" min="10" style="14" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="15" width="22.1740890688259"/>
-    <col collapsed="false" hidden="false" max="1025" min="13" style="15" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="13" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="13" width="50.9230769230769"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="13" width="22.7651821862348"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="18.3684210526316"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="13" width="17.753036437247"/>
+    <col collapsed="false" hidden="false" max="9" min="6" style="13" width="11.8744939271255"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="14" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="15" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="16" width="22.6437246963563"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="16" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="20"/>
       <c r="L1" s="0"/>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="19" t="s">
+    <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="22"/>
+      <c r="K2" s="24"/>
       <c r="L2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23" t="s">
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="E3" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F3" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I3" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="K3" s="30"/>
-      <c r="L3" s="31"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="23" t="s">
+      <c r="F3" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H3" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J3" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K3" s="32"/>
+      <c r="L3" s="33"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="25" t="n">
+      <c r="C4" s="27" t="n">
         <v>3582910032373</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="27" t="s">
+      <c r="E4" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F4" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H4" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I4" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J4" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" s="30"/>
-      <c r="L4" s="31"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="23" t="s">
+      <c r="F4" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J4" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="25" t="n">
+      <c r="C5" s="27" t="n">
         <v>3582910034988</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="28" t="s">
         <v>45</v>
       </c>
-      <c r="E5" s="27" t="s">
+      <c r="E5" s="29" t="s">
         <v>43</v>
       </c>
-      <c r="F5" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G5" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H5" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I5" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J5" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="30"/>
-      <c r="L5" s="31"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="23" t="s">
+      <c r="F5" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I5" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K5" s="32"/>
+      <c r="L5" s="33"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="25" t="s">
+      <c r="C6" s="27" t="s">
         <v>48</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F6" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G6" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H6" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I6" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J6" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="K6" s="30"/>
-      <c r="L6" s="31"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="23" t="s">
+      <c r="F6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I6" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J6" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K6" s="32"/>
+      <c r="L6" s="33"/>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="25" t="n">
+      <c r="C7" s="27" t="n">
         <v>201513619</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="28" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I7" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J7" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="30"/>
-      <c r="L7" s="31"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="23" t="s">
+      <c r="F7" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I7" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J7" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K7" s="32"/>
+      <c r="L7" s="33"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="26" t="s">
         <v>53</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E8" s="26" t="s">
+      <c r="E8" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H8" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I8" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J8" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="31"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="23" t="s">
+      <c r="F8" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I8" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J8" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K8" s="32"/>
+      <c r="L8" s="33"/>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="25" t="s">
+      <c r="C9" s="27" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="26" t="s">
+      <c r="D9" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="26" t="s">
+      <c r="E9" s="28" t="s">
         <v>56</v>
       </c>
-      <c r="F9" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G9" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H9" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I9" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J9" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="31"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="23" t="s">
+      <c r="F9" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H9" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I9" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J9" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K9" s="32"/>
+      <c r="L9" s="33"/>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="26" t="s">
+      <c r="D10" s="28" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="26" t="s">
+      <c r="E10" s="28" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G10" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H10" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I10" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J10" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="31"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="23" t="s">
+      <c r="F10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I10" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J10" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K10" s="32"/>
+      <c r="L10" s="33"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C11" s="25" t="s">
+      <c r="C11" s="27" t="s">
         <v>64</v>
       </c>
-      <c r="D11" s="32" t="s">
+      <c r="D11" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E11" s="26" t="s">
+      <c r="E11" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G11" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H11" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I11" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="J11" s="29" t="n">
-        <v>1</v>
-      </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="31"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="23" t="s">
+      <c r="F11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I11" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="J11" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="K11" s="32"/>
+      <c r="L11" s="33"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C12" s="25" t="s">
+      <c r="C12" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="D12" s="32" t="s">
+      <c r="D12" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E12" s="26" t="s">
+      <c r="E12" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="F12" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="G12" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" s="28" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" s="28" t="n">
-        <v>0</v>
-      </c>
-      <c r="J12" s="29" t="n">
-        <v>0</v>
-      </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="31"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I13" s="33"/>
-      <c r="J13" s="34"/>
+      <c r="F12" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="30" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" s="30" t="n">
+        <v>0</v>
+      </c>
+      <c r="J12" s="31" t="n">
+        <v>0</v>
+      </c>
+      <c r="K12" s="32"/>
+      <c r="L12" s="33"/>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I13" s="35"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2315,110 +2322,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="35" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="35" width="31.3846153846154"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="35" width="21.3157894736842"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="35" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="36" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="15" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="25.82995951417"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="36" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="36" width="32.0728744939271"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="36" width="21.914979757085"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="36" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="37" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="16" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="17" t="s">
+      <c r="A1" s="38"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="39" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="38"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="38"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="41"/>
-      <c r="D4" s="42"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="38"/>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="42"/>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="38"/>
-      <c r="B6" s="41"/>
-      <c r="C6" s="41"/>
-      <c r="D6" s="42"/>
-      <c r="F6" s="28"/>
-      <c r="G6" s="28"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="28"/>
-    </row>
+    <row r="1048558" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048559" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048560" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048561" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048562" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048563" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048564" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048565" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048566" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048567" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048568" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048569" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
@@ -2441,242 +2426,242 @@
   </sheetPr>
   <dimension ref="A1:J37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="43" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="43" width="19.7085020242915"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="44" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="43" width="49.2753036437247"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="43" width="34.7085020242915"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="43" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="45" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="45" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="40" width="21.3036437246964"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="40" width="20.1943319838057"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="41" width="21.3036437246964"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="40" width="50.4372469635628"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="40" width="35.6194331983806"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="40" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="42" width="10.5263157894737"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="42" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="17" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="19" t="s">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="22" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="H3" s="40"/>
+      <c r="I3" s="40"/>
+      <c r="J3" s="40"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H4" s="43"/>
-      <c r="I4" s="43"/>
-      <c r="J4" s="43"/>
+      <c r="H4" s="40"/>
+      <c r="I4" s="40"/>
+      <c r="J4" s="40"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H5" s="43"/>
-      <c r="I5" s="43"/>
-      <c r="J5" s="43"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="40"/>
+      <c r="J5" s="40"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="40"/>
+      <c r="J6" s="40"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H7" s="43"/>
-      <c r="I7" s="43"/>
-      <c r="J7" s="43"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="40"/>
+      <c r="J7" s="40"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H8" s="43"/>
-      <c r="I8" s="43"/>
-      <c r="J8" s="43"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="40"/>
+      <c r="J8" s="40"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H9" s="43"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="43"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="40"/>
+      <c r="J9" s="40"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+      <c r="H10" s="40"/>
+      <c r="I10" s="40"/>
+      <c r="J10" s="40"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H11" s="43"/>
-      <c r="I11" s="43"/>
-      <c r="J11" s="43"/>
+      <c r="H11" s="40"/>
+      <c r="I11" s="40"/>
+      <c r="J11" s="40"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H12" s="43"/>
-      <c r="I12" s="43"/>
-      <c r="J12" s="43"/>
+      <c r="H12" s="40"/>
+      <c r="I12" s="40"/>
+      <c r="J12" s="40"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H13" s="43"/>
-      <c r="I13" s="43"/>
-      <c r="J13" s="43"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="40"/>
+      <c r="J13" s="40"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H14" s="43"/>
-      <c r="I14" s="43"/>
-      <c r="J14" s="43"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="40"/>
+      <c r="J15" s="40"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H16" s="43"/>
-      <c r="I16" s="43"/>
-      <c r="J16" s="43"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H17" s="43"/>
-      <c r="I17" s="43"/>
-      <c r="J17" s="43"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
+      <c r="H19" s="40"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
+      <c r="H20" s="40"/>
+      <c r="I20" s="40"/>
+      <c r="J20" s="40"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="40"/>
+      <c r="J22" s="40"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
+      <c r="H24" s="40"/>
+      <c r="I24" s="40"/>
+      <c r="J24" s="40"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
+      <c r="H25" s="40"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
+      <c r="H26" s="40"/>
+      <c r="I26" s="40"/>
+      <c r="J26" s="40"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H27" s="43"/>
-      <c r="I27" s="43"/>
-      <c r="J27" s="43"/>
+      <c r="H27" s="40"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="H28" s="40"/>
+      <c r="I28" s="40"/>
+      <c r="J28" s="40"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="H29" s="40"/>
+      <c r="I29" s="40"/>
+      <c r="J29" s="40"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H30" s="43"/>
-      <c r="I30" s="43"/>
-      <c r="J30" s="43"/>
+      <c r="H30" s="40"/>
+      <c r="I30" s="40"/>
+      <c r="J30" s="40"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
+      <c r="H31" s="40"/>
+      <c r="I31" s="40"/>
+      <c r="J31" s="40"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H32" s="43"/>
-      <c r="I32" s="43"/>
-      <c r="J32" s="43"/>
+      <c r="H32" s="40"/>
+      <c r="I32" s="40"/>
+      <c r="J32" s="40"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H33" s="43"/>
-      <c r="I33" s="43"/>
-      <c r="J33" s="43"/>
+      <c r="H33" s="40"/>
+      <c r="I33" s="40"/>
+      <c r="J33" s="40"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H34" s="43"/>
-      <c r="I34" s="43"/>
-      <c r="J34" s="43"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="40"/>
+      <c r="J34" s="40"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H35" s="43"/>
-      <c r="I35" s="43"/>
-      <c r="J35" s="43"/>
+      <c r="H35" s="40"/>
+      <c r="I35" s="40"/>
+      <c r="J35" s="40"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H36" s="43"/>
-      <c r="I36" s="43"/>
-      <c r="J36" s="43"/>
+      <c r="H36" s="40"/>
+      <c r="I36" s="40"/>
+      <c r="J36" s="40"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H37" s="43"/>
-      <c r="I37" s="43"/>
-      <c r="J37" s="43"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2698,71 +2683,72 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E5" activeCellId="0" sqref="E5"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="35" width="28.7085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="47" width="32.5627530364372"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="35" width="30.2064777327935"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="47" width="26.5668016194332"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="47" width="18.9595141700405"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="35" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="36" width="10.9271255060729"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="48" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="36" width="29.3805668016194"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="44" width="33.4210526315789"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="36" width="30.9716599190283"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="44" width="27.2995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="44" width="19.4655870445344"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="36" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="37" width="11.1417004048583"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="45" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="46" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="16"/>
-      <c r="B1" s="16"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="17" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="0"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="49" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="49" t="s">
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="47"/>
+    </row>
+    <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="48" t="s">
         <v>31</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="49" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="50" t="s">
         <v>20</v>
       </c>
@@ -2794,7 +2780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="50" t="s">
         <v>20</v>
       </c>
@@ -2826,7 +2812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="50" t="s">
         <v>20</v>
       </c>
@@ -2858,7 +2844,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="28.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="14.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="50" t="s">
         <v>20</v>
       </c>
@@ -2890,12 +2876,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F1:I1"/>
@@ -2925,20 +2905,20 @@
   <dimension ref="A1:J80"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="56" width="31.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="56" width="43.4898785425101"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="57" width="18.8542510121457"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="57" width="17.6761133603239"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="57" width="27.7449392712551"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="57" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="58" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="58" width="8.89068825910931"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="59" width="8.89068825910931"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="56" width="32.1983805668016"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="56" width="44.5627530364373"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="57" width="19.3441295546559"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="57" width="17.995951417004"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="57" width="28.4008097165992"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="57" width="9.54655870445344"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="58" width="9.54655870445344"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="58" width="9.06072874493927"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="59" width="9.06072874493927"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2947,12 +2927,12 @@
       <c r="C1" s="60"/>
       <c r="D1" s="60"/>
       <c r="E1" s="60"/>
-      <c r="F1" s="17" t="s">
+      <c r="F1" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2965,29 +2945,29 @@
       <c r="C2" s="61" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="49" t="s">
+      <c r="E2" s="48" t="s">
         <v>34</v>
       </c>
-      <c r="F2" s="20" t="s">
+      <c r="F2" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="G2" s="20" t="s">
+      <c r="G2" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="H2" s="20" t="s">
+      <c r="H2" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="20" t="s">
+      <c r="I2" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="J2" s="20" t="s">
+      <c r="J2" s="22" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="62" t="s">
         <v>12</v>
       </c>
@@ -3019,7 +2999,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="62" t="s">
         <v>12</v>
       </c>
@@ -3051,7 +3031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="62" t="s">
         <v>12</v>
       </c>
@@ -3083,7 +3063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="62" t="s">
         <v>12</v>
       </c>
@@ -3115,7 +3095,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="62" t="s">
         <v>12</v>
       </c>
@@ -3147,7 +3127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="62" t="s">
         <v>12</v>
       </c>
@@ -3179,7 +3159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="62" t="s">
         <v>12</v>
       </c>
@@ -3211,7 +3191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="62" t="s">
         <v>12</v>
       </c>
@@ -3243,7 +3223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="62" t="s">
         <v>12</v>
       </c>
@@ -3275,7 +3255,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="62" t="s">
         <v>12</v>
       </c>
@@ -3307,7 +3287,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="70" t="s">
         <v>22</v>
       </c>
@@ -3339,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="70" t="s">
         <v>22</v>
       </c>
@@ -3371,7 +3351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="70" t="s">
         <v>22</v>
       </c>
@@ -3403,7 +3383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="70" t="s">
         <v>22</v>
       </c>

</xml_diff>